<commit_message>
update with changes for publication
</commit_message>
<xml_diff>
--- a/results/correlations.xlsx
+++ b/results/correlations.xlsx
@@ -396,16 +396,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.3330576232498121</v>
+        <v>-0.2407239916940589</v>
       </c>
       <c r="C2">
-        <v>0.01641443675541925</v>
+        <v>0.009033579491229321</v>
       </c>
       <c r="D2">
-        <v>-0.3330853049508674</v>
+        <v>-0.2423913045098955</v>
       </c>
       <c r="E2">
-        <v>-0.3330299409746317</v>
+        <v>-0.2390552569459463</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -420,16 +420,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.3219019945428436</v>
+        <v>-0.5803439289158613</v>
       </c>
       <c r="C3">
-        <v>0.08965355917815478</v>
+        <v>0.03274360758043506</v>
       </c>
       <c r="D3">
-        <v>-0.3220548208526465</v>
+        <v>-0.5845858438557359</v>
       </c>
       <c r="E3">
-        <v>-0.3217491514563667</v>
+        <v>-0.5760702868730736</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -444,16 +444,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.2397898443803017</v>
+        <v>-0.1859378220230946</v>
       </c>
       <c r="C4">
-        <v>0.008615565427009234</v>
+        <v>0.005112071127402038</v>
       </c>
       <c r="D4">
-        <v>-0.2398052461143129</v>
+        <v>-0.1869049750396768</v>
       </c>
       <c r="E4">
-        <v>-0.2397744425255866</v>
+        <v>-0.1849703085686199</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.3330576232498121</v>
+        <v>-0.2407239916940589</v>
       </c>
       <c r="C5">
-        <v>0.01641443675541925</v>
+        <v>0.009033579491229321</v>
       </c>
       <c r="D5">
-        <v>-0.3330853049508674</v>
+        <v>-0.2423913045098955</v>
       </c>
       <c r="E5">
-        <v>-0.3330299409746317</v>
+        <v>-0.2390552569459463</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.2424072198799316</v>
+        <v>-0.4513711966981849</v>
       </c>
       <c r="C6">
-        <v>0.06344314953368604</v>
+        <v>0.02166622749986542</v>
       </c>
       <c r="D6">
-        <v>-0.242520629681804</v>
+        <v>-0.4547466340866235</v>
       </c>
       <c r="E6">
-        <v>-0.2422938034528087</v>
+        <v>-0.4479827925341042</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -516,16 +516,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>-0.1440401016173417</v>
+        <v>-0.1549396964772941</v>
       </c>
       <c r="C7">
-        <v>0.00872373879828346</v>
+        <v>0.003963964878086172</v>
       </c>
       <c r="D7">
-        <v>-0.1440563048754733</v>
+        <v>-0.1556978947484505</v>
       </c>
       <c r="E7">
-        <v>-0.1440238982819731</v>
+        <v>-0.1541813156418506</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>

</xml_diff>